<commit_message>
Add profiles data for Forni
</commit_message>
<xml_diff>
--- a/Input/Lyr/profile/LYR_OM_profile.xlsx
+++ b/Input/Lyr/profile/LYR_OM_profile.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f313c7e1df1b448f/Nauka/Projekty/W trakcie/OPUS_Biomass related to animals in cryoconite holes/Statystyka/Input/Lyr/profile/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adm\OneDrive\Nauka\Projekty\W trakcie\OPUS_Effects of animals on oxygen conditions in cryoconite holes\Effects-of-animals-on-oxygen-conditions-in-cryoconite-holes\Input\Lyr\profile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="11_F25DC773A252ABDACC104879419854645ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31A5401D-4B2C-43B7-9143-ACD3D6E497F6}"/>
   <bookViews>
-    <workbookView xWindow="1416" yWindow="996" windowWidth="21624" windowHeight="11244" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1410" yWindow="990" windowWidth="21630" windowHeight="11250"/>
   </bookViews>
   <sheets>
     <sheet name="Dane" sheetId="1" r:id="rId1"/>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -371,16 +370,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -394,7 +393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -408,7 +407,7 @@
         <v>6.02</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -422,7 +421,7 @@
         <v>6.74</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -436,7 +435,7 @@
         <v>10.01</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -450,7 +449,7 @@
         <v>5.56</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -464,7 +463,7 @@
         <v>5.74</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>

</xml_diff>